<commit_message>
Code finished and Project most finished
</commit_message>
<xml_diff>
--- a/Project1/Docs/Demographics_base (version 1).xlsx
+++ b/Project1/Docs/Demographics_base (version 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="0" windowWidth="13820" windowHeight="14400" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1460" yWindow="0" windowWidth="11560" windowHeight="14840" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="demograph_base (2)" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="336">
   <si>
     <t>Variable</t>
   </si>
@@ -631,10 +631,6 @@
 n=502</t>
   </si>
   <si>
-    <t>No Hard Drug Use
-n=472</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -648,9 +644,6 @@
   </si>
   <si>
     <t>185 (36.85)</t>
-  </si>
-  <si>
-    <t>Smoker</t>
   </si>
   <si>
     <t>Never/Former</t>
@@ -699,9 +692,6 @@
     <t>20 (51.28)</t>
   </si>
   <si>
-    <t>Alcohol Use</t>
-  </si>
-  <si>
     <t>&lt;13 drinks/week</t>
   </si>
   <si>
@@ -768,9 +758,6 @@
     <t>163 (36.55)</t>
   </si>
   <si>
-    <t>Adherence</t>
-  </si>
-  <si>
     <t>95-100%</t>
   </si>
   <si>
@@ -921,9 +908,6 @@
     <t>Base Estimate</t>
   </si>
   <si>
-    <t>2Year Estimates</t>
-  </si>
-  <si>
     <t>Non-Hard Drug Use</t>
   </si>
   <si>
@@ -963,15 +947,9 @@
     <t>Crude Model (0.0851)</t>
   </si>
   <si>
-    <t>21.2223098 (3.43691524)</t>
-  </si>
-  <si>
     <t>&lt;.0001</t>
   </si>
   <si>
-    <t>-2.53247472 (1.35931258 )</t>
-  </si>
-  <si>
     <t>Aggregate Mental Health Change</t>
   </si>
   <si>
@@ -981,12 +959,6 @@
     <t>1.43 (2.01)</t>
   </si>
   <si>
-    <t>23.19 (2.72)</t>
-  </si>
-  <si>
-    <t>-0.02 (1.72)</t>
-  </si>
-  <si>
     <t>Viral Load Change</t>
   </si>
   <si>
@@ -996,25 +968,74 @@
     <t>0.01 (0.21)</t>
   </si>
   <si>
-    <t>-.1164727595 (0.43)</t>
-  </si>
-  <si>
-    <t>-0.07 (0.2)</t>
-  </si>
-  <si>
-    <t>CD4 cell count Change</t>
-  </si>
-  <si>
     <t>182.5969476 (8.43)</t>
   </si>
   <si>
     <t>-169.16 (29.68)</t>
   </si>
   <si>
-    <t>243.24 (45.86)</t>
-  </si>
-  <si>
-    <t>-157.85 (30.29)</t>
+    <t>-3.2155138 (1.4)</t>
+  </si>
+  <si>
+    <t>16.714 (3.69)</t>
+  </si>
+  <si>
+    <t>20.919 (3.126)</t>
+  </si>
+  <si>
+    <t>-0.55 (1.77)</t>
+  </si>
+  <si>
+    <t>0.348 (.459)</t>
+  </si>
+  <si>
+    <t>-0.0122 (0.2)</t>
+  </si>
+  <si>
+    <t>169.724 (52.76)</t>
+  </si>
+  <si>
+    <t>-166.61 (31.25)</t>
+  </si>
+  <si>
+    <t>2Year Change Estimates (adjusted)</t>
+  </si>
+  <si>
+    <t>Age (SD)</t>
+  </si>
+  <si>
+    <t>BMI (SD)</t>
+  </si>
+  <si>
+    <t>Education (%)</t>
+  </si>
+  <si>
+    <t>Race (%)</t>
+  </si>
+  <si>
+    <t>Income (%)</t>
+  </si>
+  <si>
+    <t>Alcohol Use (%)</t>
+  </si>
+  <si>
+    <t>Adherence (%)</t>
+  </si>
+  <si>
+    <t>Smoker (%)</t>
+  </si>
+  <si>
+    <t>Marijuana/Hash Use- Yes (%)</t>
+  </si>
+  <si>
+    <t>Non-Hard Drug Use
+n=472</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>CD4 Cell Count Change</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1098,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1085,8 +1106,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1108,8 +1181,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1127,14 +1240,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1145,6 +1294,26 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1155,6 +1324,26 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1182,11 +1371,11 @@
   <tableColumns count="5">
     <tableColumn id="1" name="Variable"/>
     <tableColumn id="2" name="Overall_x000a_n=502"/>
-    <tableColumn id="3" name="No Hard Drug Use_x000a_n=472"/>
+    <tableColumn id="3" name="Non-Hard Drug Use_x000a_n=472"/>
     <tableColumn id="4" name="Hard Drug Use _x000a_n=39"/>
     <tableColumn id="5" name="Column1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
@@ -1559,72 +1748,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="A1:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" hidden="1">
       <c r="A2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:5" hidden="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1632,79 +1821,79 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" hidden="1">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>325</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>326</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1712,35 +1901,35 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>55</v>
+        <v>327</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1751,32 +1940,32 @@
         <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1788,49 +1977,49 @@
         <v>86</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>223</v>
+        <v>329</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1839,37 +2028,37 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>246</v>
+        <v>330</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1878,67 +2067,67 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" hidden="1">
       <c r="A28" t="s">
         <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>207</v>
+        <v>331</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1947,16 +2136,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1965,28 +2154,28 @@
         <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>159</v>
+        <v>332</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1995,13 +2184,13 @@
         <v>163</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -2010,13 +2199,13 @@
         <v>164</v>
       </c>
       <c r="B34" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -2025,13 +2214,13 @@
         <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -2040,13 +2229,13 @@
         <v>166</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E36" s="1"/>
     </row>
@@ -2064,10 +2253,10 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
+        <v>201</v>
+      </c>
+      <c r="F38" t="s">
         <v>202</v>
-      </c>
-      <c r="F38" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2265,7 +2454,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D7" sqref="C3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3175,10 +3364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3190,62 +3379,118 @@
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:8">
+      <c r="B1" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>295</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="F3" s="12">
+        <f>169.724-166.61</f>
+        <v>3.1139999999999759</v>
+      </c>
+      <c r="G3">
+        <f>376.91+169.724</f>
+        <v>546.63400000000001</v>
+      </c>
+      <c r="H3">
+        <f>379.03+3.114</f>
+        <v>382.14399999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>296</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="6">
+        <f>0.348 -0.0122</f>
+        <v>0.33579999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>297</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F5" s="6">
+        <f>20.919 - 0.55</f>
+        <v>20.369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>298</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="F6" s="6">
+        <f>16.714 -3.215</f>
+        <v>13.498999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3262,219 +3507,247 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C19" sqref="C19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" s="10" customFormat="1">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="19">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="19">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="20">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" s="10" customFormat="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0.47110000000000002</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.7571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="D2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="C3">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" s="10" customFormat="1">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="C14" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E14" s="21">
+        <v>0.44829999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="C15" s="19">
+        <v>0.9446</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0.95189999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:5" s="10" customFormat="1">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="B4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4">
-        <v>8.5099999999999995E-2</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E4" s="6">
-        <v>6.3100000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="9" t="s">
+      <c r="C19" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="E19" s="20">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" t="s">
-        <v>310</v>
-      </c>
-      <c r="D8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>307</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="C9">
-        <v>1E-4</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>305</v>
-      </c>
-      <c r="B10" t="s">
-        <v>316</v>
-      </c>
-      <c r="C10">
-        <v>0.47110000000000002</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.99119999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>310</v>
-      </c>
-      <c r="D13" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>307</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="C14" t="s">
-        <v>312</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C20" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="E14" s="6">
-        <v>0.7843</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B15" t="s">
-        <v>321</v>
-      </c>
-      <c r="C15">
-        <v>0.9446</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.71830000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>310</v>
-      </c>
-      <c r="D18" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>307</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C19" t="s">
-        <v>312</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>305</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="C20" t="s">
-        <v>312</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>312</v>
+      <c r="E20" s="20" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>